<commit_message>
added scripts for event annotation
</commit_message>
<xml_diff>
--- a/data/annotation/poverty_annotation.xlsx
+++ b/data/annotation/poverty_annotation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="0" windowWidth="25540" windowHeight="19800" tabRatio="500"/>
+    <workbookView xWindow="16560" yWindow="-19940" windowWidth="22940" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="82">
   <si>
     <t>Media</t>
   </si>
@@ -84,9 +84,6 @@
     <t>http://t.co/BaH1XrS5</t>
   </si>
   <si>
-    <t>Food safety China</t>
-  </si>
-  <si>
     <t>Global food prices sharply rebound in July due to extreme weather conditions</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t xml:space="preserve">Food Health &amp; Fod Thought (religion) </t>
   </si>
   <si>
-    <t>Rising Food Prices</t>
-  </si>
-  <si>
     <t xml:space="preserve">NiallOfficial: Don the driver lovin his cup of tea! </t>
   </si>
   <si>
@@ -259,6 +253,18 @@
   </si>
   <si>
     <t>Economic Access &amp; Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rising Food Prices - </t>
+  </si>
+  <si>
+    <t>http://www.cnbc.com/id/101588110</t>
+  </si>
+  <si>
+    <t>No cleawr topic</t>
+  </si>
+  <si>
+    <t>http://www.theguardian.com/society/2013/dec/17/government-under-fire-eu-funding-food-banks</t>
   </si>
 </sst>
 </file>
@@ -307,7 +313,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -327,12 +333,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="19"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +359,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,13 +691,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88:G100"/>
+    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
+    <col min="2" max="2" width="81.33203125" customWidth="1"/>
     <col min="5" max="5" width="24.1640625" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" customWidth="1"/>
     <col min="7" max="7" width="45.1640625" customWidth="1"/>
@@ -708,10 +717,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -725,10 +734,10 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -742,10 +751,10 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -762,10 +771,10 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -779,10 +788,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -796,10 +805,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -813,10 +822,10 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -833,10 +842,10 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -850,10 +859,10 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -870,10 +879,10 @@
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -887,10 +896,10 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -904,13 +913,13 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -924,10 +933,10 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -941,10 +950,10 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -958,10 +967,10 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -978,10 +987,10 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:7">
@@ -995,10 +1004,10 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -1012,10 +1021,10 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -1029,10 +1038,10 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -1046,10 +1055,10 @@
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -1066,15 +1075,15 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1">
         <v>41085</v>
@@ -1083,13 +1092,13 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:7">
@@ -1103,10 +1112,10 @@
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:7">
@@ -1120,15 +1129,15 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1">
         <v>41130</v>
@@ -1137,18 +1146,18 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1">
         <v>41142</v>
@@ -1157,15 +1166,15 @@
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1">
         <v>41150</v>
@@ -1174,15 +1183,15 @@
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1">
         <v>41151</v>
@@ -1191,18 +1200,18 @@
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1">
         <v>41156</v>
@@ -1211,10 +1220,10 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="2:7">
@@ -1228,15 +1237,15 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="2:7">
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="1">
         <v>41177</v>
@@ -1245,13 +1254,13 @@
         <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:7">
@@ -1265,15 +1274,15 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1">
         <v>41208</v>
@@ -1282,10 +1291,10 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -1299,15 +1308,15 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1">
         <v>41246</v>
@@ -1316,15 +1325,15 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="1">
         <v>41253</v>
@@ -1333,15 +1342,15 @@
         <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:7">
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1">
         <v>41256</v>
@@ -1350,10 +1359,10 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="2:7">
@@ -1367,15 +1376,15 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1">
         <v>41286</v>
@@ -1384,10 +1393,10 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="2:7">
@@ -1401,15 +1410,15 @@
         <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1">
         <v>41298</v>
@@ -1418,15 +1427,15 @@
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" s="1">
         <v>41303</v>
@@ -1435,10 +1444,10 @@
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:7">
@@ -1452,15 +1461,15 @@
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" s="1">
         <v>41324</v>
@@ -1469,10 +1478,10 @@
         <v>4</v>
       </c>
       <c r="F44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="2:7">
@@ -1486,10 +1495,10 @@
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G45" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="2:7">
@@ -1503,15 +1512,15 @@
         <v>4</v>
       </c>
       <c r="F46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C47" s="1">
         <v>41353</v>
@@ -1520,10 +1529,10 @@
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="2:7">
@@ -1537,15 +1546,15 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="2:7">
       <c r="B49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C49" s="1">
         <v>41401</v>
@@ -1554,15 +1563,15 @@
         <v>4</v>
       </c>
       <c r="F49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="2:7">
       <c r="B50" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C50" s="1">
         <v>41402</v>
@@ -1571,10 +1580,10 @@
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="2:7">
@@ -1588,15 +1597,15 @@
         <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G51" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="2:7">
       <c r="B52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C52" s="1">
         <v>41425</v>
@@ -1605,10 +1614,10 @@
         <v>4</v>
       </c>
       <c r="F52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G52" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="2:7">
@@ -1622,10 +1631,10 @@
         <v>4</v>
       </c>
       <c r="F53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="2:7">
@@ -1639,10 +1648,10 @@
         <v>4</v>
       </c>
       <c r="F54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="2:7">
@@ -1656,10 +1665,10 @@
         <v>4</v>
       </c>
       <c r="F55" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="2:7">
@@ -1673,10 +1682,10 @@
         <v>4</v>
       </c>
       <c r="F56" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G56" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="2:7">
@@ -1690,10 +1699,10 @@
         <v>4</v>
       </c>
       <c r="F57" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="2:7">
@@ -1707,15 +1716,15 @@
         <v>4</v>
       </c>
       <c r="F58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="2:7">
       <c r="B59" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C59" s="1">
         <v>41458</v>
@@ -1724,10 +1733,10 @@
         <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="2:7">
@@ -1741,15 +1750,15 @@
         <v>4</v>
       </c>
       <c r="F60" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="B61" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C61" s="1">
         <v>41479</v>
@@ -1758,10 +1767,10 @@
         <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="2:7">
@@ -1775,10 +1784,10 @@
         <v>4</v>
       </c>
       <c r="F62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="2:7">
@@ -1792,15 +1801,15 @@
         <v>4</v>
       </c>
       <c r="F63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="2:7">
       <c r="B64" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C64" s="1">
         <v>41494</v>
@@ -1809,10 +1818,10 @@
         <v>4</v>
       </c>
       <c r="F64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G64" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="2:7">
@@ -1826,10 +1835,10 @@
         <v>4</v>
       </c>
       <c r="F65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="2:7">
@@ -1843,10 +1852,10 @@
         <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:7">
@@ -1860,15 +1869,15 @@
         <v>4</v>
       </c>
       <c r="F67" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="2:7">
       <c r="B68" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C68" s="1">
         <v>41548</v>
@@ -1877,15 +1886,15 @@
         <v>4</v>
       </c>
       <c r="F68" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="2:7">
       <c r="B69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C69" s="1">
         <v>41556</v>
@@ -1894,15 +1903,15 @@
         <v>4</v>
       </c>
       <c r="F69" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G69" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="2:7">
       <c r="B70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C70" s="1">
         <v>41561</v>
@@ -1911,15 +1920,15 @@
         <v>4</v>
       </c>
       <c r="F70" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="2:7">
       <c r="B71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C71" s="1">
         <v>41563</v>
@@ -1928,15 +1937,15 @@
         <v>4</v>
       </c>
       <c r="F71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G71" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="2:7">
       <c r="B72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C72" s="1">
         <v>41564</v>
@@ -1945,15 +1954,15 @@
         <v>4</v>
       </c>
       <c r="F72" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="2:7">
       <c r="B73" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C73" s="1">
         <v>41585</v>
@@ -1962,15 +1971,15 @@
         <v>4</v>
       </c>
       <c r="F73" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="2:7">
       <c r="B74" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C74" s="1">
         <v>41606</v>
@@ -1979,15 +1988,15 @@
         <v>4</v>
       </c>
       <c r="F74" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="2:7">
       <c r="B75" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C75" s="1">
         <v>41618</v>
@@ -1996,15 +2005,15 @@
         <v>4</v>
       </c>
       <c r="F75" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G75" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="2:7">
       <c r="B76" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C76" s="1">
         <v>41627</v>
@@ -2012,16 +2021,19 @@
       <c r="D76" t="s">
         <v>4</v>
       </c>
+      <c r="E76" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G76" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="2:7">
       <c r="B77" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C77" s="1">
         <v>41681</v>
@@ -2030,10 +2042,10 @@
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G77" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="2:7">
@@ -2047,15 +2059,15 @@
         <v>4</v>
       </c>
       <c r="F78" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:7">
       <c r="B79" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C79" s="1">
         <v>41683</v>
@@ -2064,15 +2076,15 @@
         <v>4</v>
       </c>
       <c r="F79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="2:7">
       <c r="B80" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C80" s="1">
         <v>41702</v>
@@ -2081,10 +2093,10 @@
         <v>4</v>
       </c>
       <c r="F80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G80" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="2:7">
@@ -2098,10 +2110,10 @@
         <v>4</v>
       </c>
       <c r="F81" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G81" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="2:7">
@@ -2115,15 +2127,15 @@
         <v>4</v>
       </c>
       <c r="F82" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G82" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="2:7">
       <c r="B83" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C83" s="1">
         <v>41715</v>
@@ -2132,10 +2144,10 @@
         <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G83" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="2:7">
@@ -2149,15 +2161,15 @@
         <v>4</v>
       </c>
       <c r="F84" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G84" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="2:7">
       <c r="B85" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C85" s="1">
         <v>41743</v>
@@ -2166,10 +2178,10 @@
         <v>4</v>
       </c>
       <c r="F85" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G85" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="2:7">
@@ -2183,15 +2195,15 @@
         <v>4</v>
       </c>
       <c r="F86" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G86" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="2:7">
       <c r="B87" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C87" s="1">
         <v>41745</v>
@@ -2199,16 +2211,19 @@
       <c r="D87" t="s">
         <v>4</v>
       </c>
+      <c r="E87" t="s">
+        <v>79</v>
+      </c>
       <c r="F87" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G87" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="2:7">
       <c r="B88" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C88" s="1">
         <v>41749</v>
@@ -2217,10 +2232,10 @@
         <v>4</v>
       </c>
       <c r="F88" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G88" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="2:7">
@@ -2234,15 +2249,15 @@
         <v>4</v>
       </c>
       <c r="F89" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G89" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="2:7">
       <c r="B90" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C90" s="1">
         <v>41771</v>
@@ -2251,15 +2266,15 @@
         <v>4</v>
       </c>
       <c r="F90" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G90" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="2:7">
       <c r="B91" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C91" s="1">
         <v>41772</v>
@@ -2268,15 +2283,15 @@
         <v>4</v>
       </c>
       <c r="F91" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G91" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="2:7">
       <c r="B92" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C92" s="1">
         <v>41801</v>
@@ -2285,15 +2300,15 @@
         <v>4</v>
       </c>
       <c r="F92" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G92" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="2:7">
       <c r="B93" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C93" s="1">
         <v>41815</v>
@@ -2302,15 +2317,15 @@
         <v>4</v>
       </c>
       <c r="F93" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="2:7">
       <c r="B94" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C94" s="1">
         <v>41849</v>
@@ -2319,15 +2334,15 @@
         <v>4</v>
       </c>
       <c r="F94" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G94" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="2:7">
       <c r="B95" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C95" s="1">
         <v>41850</v>
@@ -2336,10 +2351,10 @@
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G95" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="2:7">
@@ -2353,15 +2368,15 @@
         <v>4</v>
       </c>
       <c r="F96" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G96" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="2:7">
       <c r="B97" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C97" s="1">
         <v>41890</v>
@@ -2370,15 +2385,15 @@
         <v>4</v>
       </c>
       <c r="F97" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G97" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="2:7">
       <c r="B98" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C98" s="1">
         <v>41891</v>
@@ -2387,15 +2402,15 @@
         <v>4</v>
       </c>
       <c r="F98" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G98" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="2:7">
       <c r="B99" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C99" s="1">
         <v>41892</v>
@@ -2404,15 +2419,15 @@
         <v>4</v>
       </c>
       <c r="F99" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G99" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="2:7">
       <c r="B100" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C100" s="1">
         <v>41893</v>
@@ -2421,13 +2436,16 @@
         <v>4</v>
       </c>
       <c r="F100" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G100" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E76" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>